<commit_message>
Escalaçao do dia 24/02
</commit_message>
<xml_diff>
--- a/futeletrica.xlsx
+++ b/futeletrica.xlsx
@@ -57,10 +57,10 @@
     <t>Mensal</t>
   </si>
   <si>
-    <t>X</t>
+    <t>ARI</t>
   </si>
   <si>
-    <t>ARI</t>
+    <t>X</t>
   </si>
   <si>
     <t>BRIAN ROCHA</t>
@@ -155,10 +155,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="24">
@@ -191,29 +191,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -229,7 +206,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,6 +222,29 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,6 +261,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,7 +305,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -298,10 +313,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -315,21 +330,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,6 +351,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -358,6 +412,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,19 +459,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +477,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,109 +489,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,7 +525,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,11 +588,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -612,6 +627,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -623,15 +649,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,176 +677,159 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5740740740741" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
@@ -1194,13 +1194,11 @@
       <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="11">
         <v>52</v>
@@ -1216,7 +1214,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:6">
@@ -1256,7 +1254,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:6">
@@ -1296,7 +1294,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:6">
@@ -1317,7 +1315,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1" spans="1:6">
@@ -1338,7 +1336,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:6">
@@ -1359,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:6">
@@ -1417,9 +1415,7 @@
       <c r="E14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:6">
       <c r="A15" s="5" t="s">
@@ -1458,7 +1454,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" spans="1:6">
@@ -1479,7 +1475,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1" spans="1:6">
@@ -1500,7 +1496,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:6">
@@ -1540,7 +1536,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1" spans="1:6">
@@ -1560,7 +1556,9 @@
       <c r="E21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1" spans="1:6">
       <c r="A22" s="5" t="s">
@@ -1580,7 +1578,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:6">
@@ -1601,7 +1599,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1" spans="1:6">
@@ -1622,7 +1620,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1" spans="1:6">
@@ -1680,7 +1678,9 @@
       <c r="E27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="12"/>
+      <c r="F27" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1"/>
     <row r="29" ht="14.25" customHeight="1"/>
@@ -2651,7 +2651,7 @@
     <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:F27">
-    <sortState ref="A2:F27">
+    <sortState ref="A1:F27">
       <sortCondition ref="A1"/>
     </sortState>
     <extLst/>
@@ -2853,9 +2853,9 @@
       <c r="D9" s="8">
         <v>7.82</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="9" t="str">
         <f>VLOOKUP(A9,'Base de Craques'!A:F,6,1)</f>
-        <v>0</v>
+        <v>X</v>
       </c>
     </row>
     <row r="10" ht="14.25" hidden="1" customHeight="1" spans="1:5">
@@ -2993,9 +2993,9 @@
       <c r="D16" s="8">
         <v>6.76</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="9" t="str">
         <f>VLOOKUP(A16,'Base de Craques'!A:F,6,1)</f>
-        <v>0</v>
+        <v>X</v>
       </c>
     </row>
     <row r="17" ht="14.25" hidden="1" customHeight="1" spans="1:5">
@@ -3033,9 +3033,9 @@
       <c r="D18" s="8">
         <v>6.53</v>
       </c>
-      <c r="E18" s="9" t="str">
+      <c r="E18" s="9">
         <f>VLOOKUP(A18,'Base de Craques'!A:F,6,1)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" ht="14.25" hidden="1" customHeight="1" spans="1:5">
@@ -3053,9 +3053,9 @@
       <c r="D19" s="8">
         <v>6.53</v>
       </c>
-      <c r="E19" s="9" t="str">
+      <c r="E19" s="9">
         <f>VLOOKUP(A19,'Base de Craques'!A:F,6,1)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" ht="14.25" hidden="1" customHeight="1" spans="1:5">
@@ -3200,7 +3200,7 @@
     </row>
     <row r="27" ht="14.25" hidden="1" customHeight="1" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="6">
         <f>C27+0.1+0.1</f>

</xml_diff>